<commit_message>
initial upload to rl.beiyang.ren repo
</commit_message>
<xml_diff>
--- a/_site/script/alumni_info_phd.xlsx
+++ b/_site/script/alumni_info_phd.xlsx
@@ -1,33 +1,169 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iffyuan/Documents/Website/rl.beiyang.ren/script/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B02C7C-8061-0941-9833-892195D8BE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="30720" windowHeight="13380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>序号</t>
   </si>
   <si>
+    <t>姓名</t>
+  </si>
+  <si>
+    <t>姓名的英文拼音</t>
+  </si>
+  <si>
+    <t>入学年份</t>
+  </si>
+  <si>
+    <t>毕业年份</t>
+  </si>
+  <si>
+    <t>身份</t>
+  </si>
+  <si>
+    <t>研究方向（英文）</t>
+  </si>
+  <si>
+    <t>个人主页链接</t>
+  </si>
+  <si>
+    <t>毕业去向</t>
+  </si>
+  <si>
     <t>9、请上传图片：你的照片，最后显示的是圆形头像，因此最好1比1</t>
   </si>
   <si>
+    <t>郝晓田</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xiaotian Hao </t>
+  </si>
+  <si>
+    <t>Reinforcement Learning, Multiagent system</t>
+  </si>
+  <si>
+    <t>https://tjuhaoxiaotian.github.io/</t>
+  </si>
+  <si>
+    <t>Douyin, ByteDance</t>
+  </si>
+  <si>
+    <t>https://pubuserqiniu.paperol.cn/230948160_23_q7_1691629696SWzMKa.png?attname=23_7_IMG_20230810_090725.png&amp;e=1699771284&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:hI_GtQUbpbVYBKm9_naFNHWOpWE=</t>
+  </si>
+  <si>
+    <t>马亿</t>
+  </si>
+  <si>
+    <t>Yi Ma</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning, Embodied AI, RL for Application</t>
+  </si>
+  <si>
+    <t>https://mayi1996.top/</t>
+  </si>
+  <si>
+    <t>Associate Professor, School of Comuputer and Information Technology (School of Big Data), Shanxi University</t>
+  </si>
+  <si>
+    <t>https://pubuserqiniu.paperol.cn/230948160_2_q7_1691396847GNejty.jpg?attname=5_7_%e5%be%ae%e4%bf%a1%e5%9b%be%e7%89%87_20200401235353.jpg&amp;e=1699771284&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:GaZ5F7j59XMFMQIlmPj9GUw3ClU=</t>
+  </si>
+  <si>
+    <t>王维埙</t>
+  </si>
+  <si>
+    <t>Weixun Wang</t>
+  </si>
+  <si>
+    <t>LargeScale Multiagent Deep Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>https://wwxfromtju.github.io</t>
+  </si>
+  <si>
+    <t>Netease Fuxi AI Lab; Alibaba</t>
+  </si>
+  <si>
+    <t>https://pubuserqiniu.paperol.cn/230944298_9_q9_1691746175d8yZfA.png?attname=9_9_weixunwang.png&amp;e=1699852833&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:2v-0-q8RK2A1DkF_Ssn-ZrDhZmE=</t>
+  </si>
+  <si>
+    <t>汤宏垚</t>
+  </si>
+  <si>
+    <t>Hongyao Tang</t>
+  </si>
+  <si>
+    <t>Deep Reinforcement Learning, Representation Learning</t>
+  </si>
+  <si>
+    <t>https://bluecontra.github.io/</t>
+  </si>
+  <si>
+    <t>Postdoctoral Fellow of UdeM/MILA; Associate Reseacher, Tianjin University</t>
+  </si>
+  <si>
+    <t>https://pubuserqiniu.paperol.cn/230944298_1_q9_1691486667QWJ2sY.jpg?attname=1_9_%e5%ad%a6%e6%9c%af%e4%ba%a4%e6%b5%81%e6%9d%90%e6%96%99%e4%b8%aa%e4%ba%ba%e7%85%a7%e7%89%871-%e6%ad%a3%e6%96%b9%e5%bd%a2.jpg&amp;e=1700393119&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:pfIE4-Q6tq_xUhVHGmoHY89R1r4=</t>
+  </si>
+  <si>
+    <t>杨天培</t>
+  </si>
+  <si>
+    <t>Tianpei Yang</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning; Transfer Learning; Multiagent Learning</t>
+  </si>
+  <si>
+    <t>https://tianpeiyang.github.io/</t>
+  </si>
+  <si>
+    <t>Postdoc at University of Alberta; Associate Professor, Nanjing University</t>
+  </si>
+  <si>
+    <t>https://pubuserqiniu.paperol.cn/230944298_2_q9_1691524593CxMcAs.jpg?attname=2_9_profile.jpg&amp;e=1700393119&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:AwvHAbwQW5uA8VZ0tdNvQOAtQbE=</t>
+  </si>
+  <si>
+    <t>郑岩</t>
+  </si>
+  <si>
+    <t>Yan Zheng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiagent Systems; Deep Reinforcement Learning; Evolutionary Algorithm; </t>
+  </si>
+  <si>
+    <t>https://yanzzzzz.github.io/</t>
+  </si>
+  <si>
+    <t>Associate Professor, College of Intelligence and Computing, Tianjin University</t>
+  </si>
+  <si>
     <t>张程伟</t>
   </si>
   <si>
@@ -40,197 +176,51 @@
     <t>https://ist.dlmu.edu.cn/professor/zhangchengwei2.html</t>
   </si>
   <si>
+    <t>Associate Professor, Dalian Maritime University</t>
+  </si>
+  <si>
     <t>https://pubuserqiniu.paperol.cn/230944298_6_q9_1691650135knZhrS.jpg?attname=6_9_%e5%bc%a0%e7%a8%8b%e4%bc%9f%e4%b8%aa%e4%ba%ba%e8%af%81%e4%bb%b6%e7%85%a7%e7%89%87.jpg&amp;e=1699852833&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:rNWbratlSqJuXmoAtDTy3aOmXgg=</t>
   </si>
   <si>
-    <t>王维埙</t>
-  </si>
-  <si>
-    <t>Weixun Wang</t>
-  </si>
-  <si>
-    <t>LargeScale Multiagent Deep Reinforcement Learning</t>
-  </si>
-  <si>
-    <t>姓名</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>姓名的英文拼音</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>毕业去向</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>个人主页链接</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>研究方向（英文）</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>身份</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>入学年份</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>毕业年份</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://wwxfromtju.github.io</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>杨天培</t>
-  </si>
-  <si>
-    <t>Tianpei Yang</t>
-  </si>
-  <si>
-    <t>Reinforcement Learning; Transfer Learning; Multiagent Learning</t>
-  </si>
-  <si>
-    <t>https://tianpeiyang.github.io/</t>
-  </si>
-  <si>
-    <t>汤宏垚</t>
-  </si>
-  <si>
-    <t>Hongyao Tang</t>
-  </si>
-  <si>
-    <t>https://bluecontra.github.io/</t>
-  </si>
-  <si>
-    <t>郑岩</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>Deep Reinforcement Learning, Representation Learning</t>
-  </si>
-  <si>
-    <t>https://pubuserqiniu.paperol.cn/230944298_1_q9_1691486667QWJ2sY.jpg?attname=1_9_%e5%ad%a6%e6%9c%af%e4%ba%a4%e6%b5%81%e6%9d%90%e6%96%99%e4%b8%aa%e4%ba%ba%e7%85%a7%e7%89%871-%e6%ad%a3%e6%96%b9%e5%bd%a2.jpg&amp;e=1700393119&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:pfIE4-Q6tq_xUhVHGmoHY89R1r4=</t>
-  </si>
-  <si>
-    <t>https://pubuserqiniu.paperol.cn/230944298_2_q9_1691524593CxMcAs.jpg?attname=2_9_profile.jpg&amp;e=1700393119&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:AwvHAbwQW5uA8VZ0tdNvQOAtQbE=</t>
-  </si>
-  <si>
-    <t>https://yanzzzzz.github.io/</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiagent Systems; Deep Reinforcement Learning; Evolutionary Algorithm; </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yan Zheng</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Associate Professor, Dalian Maritime University</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Associate Professor, College of Intelligence and Computing, Tianjin University</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://pubuserqiniu.paperol.cn/230944298_9_q9_1691746175d8yZfA.png?attname=9_9_weixunwang.png&amp;e=1699852833&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:2v-0-q8RK2A1DkF_Ssn-ZrDhZmE=</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>马亿</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yi Ma</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reinforcement Learning, Embodied AI, RL for Application</t>
-  </si>
-  <si>
-    <t>https://mayi1996.top/</t>
-  </si>
-  <si>
-    <t>Associate Professor, School of Comuputer and Information Technology (School of Big Data), Shanxi University</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Netease Fuxi AI Lab; Alibaba</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://pubuserqiniu.paperol.cn/230948160_2_q7_1691396847GNejty.jpg?attname=5_7_%e5%be%ae%e4%bf%a1%e5%9b%be%e7%89%87_20200401235353.jpg&amp;e=1699771284&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:GaZ5F7j59XMFMQIlmPj9GUw3ClU=</t>
-  </si>
-  <si>
-    <t>郝晓田</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xiaotian Hao </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reinforcement Learning, Multiagent system</t>
-  </si>
-  <si>
-    <t>https://pubuserqiniu.paperol.cn/230948160_23_q7_1691629696SWzMKa.png?attname=23_7_IMG_20230810_090725.png&amp;e=1699771284&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:hI_GtQUbpbVYBKm9_naFNHWOpWE=</t>
-  </si>
-  <si>
-    <t>Douyin, ByteDance</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://tjuhaoxiaotian.github.io/</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Postdoc at University of Alberta; Associate Professor, Nanjing University</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Postdoctoral Fellow of UdeM/MILA; Associate Reseacher, Tianjin University</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>倪飞</t>
+  </si>
+  <si>
+    <t>Spike</t>
+  </si>
+  <si>
+    <t>Model based RL; Diffusion for RL; LLM</t>
+  </si>
+  <si>
+    <t>https://fei-ni.github.io</t>
+  </si>
+  <si>
+    <t>Postdoctoral fellow,Imperial College London</t>
+  </si>
+  <si>
+    <t>https://pubuserqiniu.paperol.cn/230948160_18_q7_1691566953phrMka.jpg?attname=20_7_%e8%af%81%e4%bb%b6%e7%85%a71_1.jpg&amp;e=1699771284&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:V4xgygdN3C4K0YvwD90au26bLWg=</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;¥&quot;* #,##0_ ;_ &quot;¥&quot;* \-#,##0_ ;_ &quot;¥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="6">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ \¥* #,##0.00_ ;_ \¥* \-#,##0.00_ ;_ \¥* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ \¥* #,##0_ ;_ \¥* \-#,##0_ ;_ \¥* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="24">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="宋体"/>
-      <family val="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
     </font>
     <font>
@@ -238,38 +228,359 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -277,47 +588,329 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="Comma" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Comma [0]" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Currency" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Currency [0]" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Percent" xfId="1" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+  <cellStyles count="55">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="Comma" xfId="49"/>
+    <cellStyle name="Comma [0]" xfId="50"/>
+    <cellStyle name="Currency" xfId="51"/>
+    <cellStyle name="Currency [0]" xfId="52"/>
+    <cellStyle name="Normal" xfId="53"/>
+    <cellStyle name="Percent" xfId="54"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -637,69 +1230,69 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="9.16666666666667" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" customWidth="1"/>
+    <col min="1" max="1" width="4.16666666666667" customWidth="1"/>
     <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.8333333333333" customWidth="1"/>
     <col min="4" max="5" width="9.5" customWidth="1"/>
     <col min="6" max="6" width="6.5" customWidth="1"/>
-    <col min="7" max="7" width="53.33203125" customWidth="1"/>
+    <col min="7" max="7" width="53.3333333333333" customWidth="1"/>
     <col min="8" max="8" width="46.5" customWidth="1"/>
-    <col min="9" max="9" width="46.33203125" customWidth="1"/>
-    <col min="10" max="10" width="255.6640625" customWidth="1"/>
+    <col min="9" max="9" width="46.3333333333333" customWidth="1"/>
+    <col min="10" max="10" width="255.666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="B2" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>2020</v>
@@ -711,24 +1304,24 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="14">
+    <row r="3" spans="1:10">
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D3" s="1">
         <v>2020</v>
@@ -739,25 +1332,25 @@
       <c r="F3" s="1">
         <v>2</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>39</v>
+      <c r="G3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>2019</v>
@@ -769,24 +1362,24 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D5">
         <v>2019</v>
@@ -798,24 +1391,24 @@
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="B6" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D6">
         <v>2017</v>
@@ -827,24 +1420,24 @@
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="16">
-      <c r="B7" s="3" t="s">
-        <v>26</v>
+    <row r="7" ht="15" spans="1:10">
+      <c r="B7" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D7">
         <v>2014</v>
@@ -856,21 +1449,21 @@
         <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="I7" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="B8" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="D8">
         <v>2011</v>
@@ -882,31 +1475,61 @@
         <v>2</v>
       </c>
       <c r="G8" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="H8" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>6</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" spans="1:10">
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9">
+        <v>2021</v>
+      </c>
+      <c r="E9">
+        <v>2025</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:J7">
-    <sortCondition descending="1" ref="E1"/>
+  <sortState ref="A3:J7">
+    <sortCondition ref="E1" descending="1"/>
   </sortState>
-  <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="H7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="J4" r:id="rId3" xr:uid="{CFBE7614-56FB-433A-B046-01F03BE6F362}"/>
-    <hyperlink ref="H3" r:id="rId4" xr:uid="{42C16A8A-833B-49BE-9256-10A3102BE9BB}"/>
-    <hyperlink ref="H2" r:id="rId5" xr:uid="{C704FF05-452E-45AA-BB11-6A7531531C05}"/>
+    <hyperlink ref="H4" r:id="rId1" display="https://wwxfromtju.github.io"/>
+    <hyperlink ref="H7" r:id="rId2" display="https://yanzzzzz.github.io/"/>
+    <hyperlink ref="J4" r:id="rId3" display="https://pubuserqiniu.paperol.cn/230944298_9_q9_1691746175d8yZfA.png?attname=9_9_weixunwang.png&amp;e=1699852833&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:2v-0-q8RK2A1DkF_Ssn-ZrDhZmE="/>
+    <hyperlink ref="H3" r:id="rId4" display="https://mayi1996.top/"/>
+    <hyperlink ref="H2" r:id="rId5" display="https://tjuhaoxiaotian.github.io/"/>
+    <hyperlink ref="J9" r:id="rId6" display="https://pubuserqiniu.paperol.cn/230948160_18_q7_1691566953phrMka.jpg?attname=20_7_%e8%af%81%e4%bb%b6%e7%85%a71_1.jpg&amp;e=1699771284&amp;token=-kY3jr8KMC7l3KkIN3OcIs8Q4s40OfGgUHr1Rg4D:V4xgygdN3C4K0YvwD90au26bLWg="/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>